<commit_message>
Changed the format of the contour table and adapted the functions to take this new format, fixed indexing errors in the CEAOut Function
</commit_message>
<xml_diff>
--- a/REGEN/CEA_Maelstrom.xlsx
+++ b/REGEN/CEA_Maelstrom.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="78114" uniqueCount="9968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="104152" uniqueCount="9969">
   <si>
     <t>0</t>
   </si>
@@ -29936,6 +29936,9 @@
   </si>
   <si>
     <t>2616</t>
+  </si>
+  <si>
+    <t>9e-05</t>
   </si>
 </sst>
 </file>
@@ -30400,7 +30403,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>0</v>
+        <v>9968</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>999</v>

</xml_diff>